<commit_message>
Add methods for retrieving teams and corresponding test cases
</commit_message>
<xml_diff>
--- a/TestData/test_data.xlsx
+++ b/TestData/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\asana_api_automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B8FFFA-7389-4AF4-8129-D2CC91AF30D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA254A2-1EC7-4554-A18B-45D22B538EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workSpace_data" sheetId="1" r:id="rId1"/>
+    <sheet name="teams" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>TestCase</t>
   </si>
@@ -100,13 +101,40 @@
   </si>
   <si>
     <t>/workspaces/{workspace_gid}/addUser</t>
+  </si>
+  <si>
+    <t>Teams</t>
+  </si>
+  <si>
+    <r>
+      <t>/workspaces/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{workspace_gid}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF384248"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/teams</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +162,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF384248"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -163,6 +197,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,15 +480,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.44140625" customWidth="1"/>
     <col min="7" max="7" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" customWidth="1"/>
@@ -586,4 +621,113 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D582A752-69C2-493B-BA26-B9CB8F02D21D}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="28.8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="D5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>